<commit_message>
Region code abbreviations added.
</commit_message>
<xml_diff>
--- a/ConcordanceLibrary/LabelsAndCodes/049_BaseRegionClassification.xlsx
+++ b/ConcordanceLibrary/LabelsAndCodes/049_BaseRegionClassification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwieland\Github workspace\PIOLab\ConcordanceLibrary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwieland\Github workspace\PIOLab\ConcordanceLibrary\LabelsAndCodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>Code</t>
   </si>
@@ -177,6 +177,156 @@
   </si>
   <si>
     <t>RoW Middle East</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WL</t>
+  </si>
+  <si>
+    <t>WE</t>
+  </si>
+  <si>
+    <t>WF</t>
+  </si>
+  <si>
+    <t>WM</t>
+  </si>
+  <si>
+    <t>Abbrev</t>
   </si>
 </sst>
 </file>
@@ -513,416 +663,569 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>50</v>
       </c>
+      <c r="C50" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>